<commit_message>
Updated ingredients excel sheet with current database entries
</commit_message>
<xml_diff>
--- a/documentation/ingredients.xlsx
+++ b/documentation/ingredients.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\E-commerce\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19530" windowHeight="3855"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19536" windowHeight="3852"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="64">
   <si>
     <t>ingredient_id</t>
   </si>
@@ -198,6 +199,24 @@
   </si>
   <si>
     <t>title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yukon Gold potatoes </t>
+  </si>
+  <si>
+    <t>pork shoulder</t>
+  </si>
+  <si>
+    <t>cilantro</t>
+  </si>
+  <si>
+    <t>avacado</t>
+  </si>
+  <si>
+    <t>elbow macaroni</t>
+  </si>
+  <si>
+    <t>potatoes</t>
   </si>
 </sst>
 </file>
@@ -553,21 +572,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView tabSelected="1" topLeftCell="F43" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" customWidth="1"/>
+    <col min="9" max="9" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -587,27 +606,27 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>50</v>
-      </c>
-      <c r="H2" s="1">
-        <v>4.99</v>
+      <c r="F2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="I2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -615,19 +634,19 @@
         <v>3</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H3" s="1">
         <v>4.99</v>
       </c>
       <c r="I3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -635,19 +654,19 @@
         <v>3</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G4">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H4" s="1">
         <v>4.99</v>
       </c>
       <c r="I4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -655,19 +674,19 @@
         <v>4</v>
       </c>
       <c r="F5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G5">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H5" s="1">
         <v>4.99</v>
       </c>
       <c r="I5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -675,19 +694,19 @@
         <v>5</v>
       </c>
       <c r="F6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G6">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H6" s="1">
         <v>4.99</v>
       </c>
       <c r="I6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>4</v>
       </c>
@@ -695,19 +714,19 @@
         <v>6</v>
       </c>
       <c r="F7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G7">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H7" s="1">
         <v>4.99</v>
       </c>
       <c r="I7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>5</v>
       </c>
@@ -715,19 +734,19 @@
         <v>7</v>
       </c>
       <c r="F8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G8">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H8" s="1">
         <v>4.99</v>
       </c>
       <c r="I8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>6</v>
       </c>
@@ -735,19 +754,19 @@
         <v>8</v>
       </c>
       <c r="F9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G9">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H9" s="1">
         <v>4.99</v>
       </c>
       <c r="I9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>6</v>
       </c>
@@ -755,19 +774,19 @@
         <v>8</v>
       </c>
       <c r="F10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G10">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H10" s="1">
         <v>4.99</v>
       </c>
       <c r="I10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>7</v>
       </c>
@@ -775,19 +794,19 @@
         <v>10</v>
       </c>
       <c r="F11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G11">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H11" s="1">
         <v>4.99</v>
       </c>
       <c r="I11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>8</v>
       </c>
@@ -795,19 +814,19 @@
         <v>9</v>
       </c>
       <c r="F12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G12">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H12" s="1">
         <v>4.99</v>
       </c>
       <c r="I12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>8</v>
       </c>
@@ -815,47 +834,47 @@
         <v>9</v>
       </c>
       <c r="F13">
+        <v>11</v>
+      </c>
+      <c r="G13">
+        <v>40</v>
+      </c>
+      <c r="H13" s="1">
+        <v>4.99</v>
+      </c>
+      <c r="I13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
         <v>12</v>
       </c>
-      <c r="G13">
+      <c r="F14">
+        <v>12</v>
+      </c>
+      <c r="G14">
         <v>39</v>
       </c>
-      <c r="H13" s="1">
-        <v>4.99</v>
-      </c>
-      <c r="I13" t="s">
+      <c r="H14" s="1">
+        <v>4.99</v>
+      </c>
+      <c r="I14" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>9</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15">
         <v>11</v>
       </c>
-      <c r="F14">
+      <c r="B15" t="s">
         <v>13</v>
       </c>
-      <c r="G14">
-        <v>38</v>
-      </c>
-      <c r="H14" s="1">
-        <v>4.99</v>
-      </c>
-      <c r="I14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>10</v>
-      </c>
-      <c r="B15" t="s">
-        <v>12</v>
-      </c>
       <c r="F15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G15">
         <v>37</v>
@@ -867,7 +886,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>11</v>
       </c>
@@ -875,7 +894,7 @@
         <v>13</v>
       </c>
       <c r="F16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G16">
         <v>36</v>
@@ -887,7 +906,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>11</v>
       </c>
@@ -895,7 +914,7 @@
         <v>13</v>
       </c>
       <c r="F17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G17">
         <v>35</v>
@@ -907,7 +926,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>11</v>
       </c>
@@ -915,7 +934,7 @@
         <v>13</v>
       </c>
       <c r="F18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G18">
         <v>33</v>
@@ -927,15 +946,15 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G19">
         <v>32</v>
@@ -947,15 +966,15 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="F20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G20">
         <v>31</v>
@@ -967,7 +986,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>13</v>
       </c>
@@ -975,7 +994,7 @@
         <v>37</v>
       </c>
       <c r="F21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G21">
         <v>30</v>
@@ -987,15 +1006,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="F22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G22">
         <v>29</v>
@@ -1007,7 +1026,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>13</v>
       </c>
@@ -1015,7 +1034,7 @@
         <v>15</v>
       </c>
       <c r="F23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G23">
         <v>28</v>
@@ -1027,15 +1046,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G24">
         <v>27</v>
@@ -1047,15 +1066,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="F25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G25">
         <v>26</v>
@@ -1067,15 +1086,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="F26">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G26">
         <v>25</v>
@@ -1087,15 +1106,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G27">
         <v>24</v>
@@ -1107,7 +1126,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>16</v>
       </c>
@@ -1115,7 +1134,7 @@
         <v>18</v>
       </c>
       <c r="F28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G28">
         <v>23</v>
@@ -1127,15 +1146,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B29" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G29">
         <v>22</v>
@@ -1147,15 +1166,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>17</v>
       </c>
       <c r="B30" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="F30">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G30">
         <v>21</v>
@@ -1167,15 +1186,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B31" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F31">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G31">
         <v>19</v>
@@ -1184,18 +1203,18 @@
         <v>4.99</v>
       </c>
       <c r="I31" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>19</v>
+      </c>
+      <c r="B32" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>18</v>
-      </c>
-      <c r="B32" t="s">
-        <v>20</v>
-      </c>
       <c r="F32">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G32">
         <v>18</v>
@@ -1207,15 +1226,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B33" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F33">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G33">
         <v>17</v>
@@ -1224,10 +1243,10 @@
         <v>4.99</v>
       </c>
       <c r="I33" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>21</v>
       </c>
@@ -1235,7 +1254,7 @@
         <v>22</v>
       </c>
       <c r="F34">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G34">
         <v>16</v>
@@ -1247,15 +1266,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B35" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F35">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G35">
         <v>15</v>
@@ -1264,18 +1283,18 @@
         <v>4.99</v>
       </c>
       <c r="I35" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B36" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F36">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G36">
         <v>14</v>
@@ -1287,15 +1306,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B37" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F37">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G37">
         <v>13</v>
@@ -1307,15 +1326,15 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B38" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F38">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G38">
         <v>12</v>
@@ -1327,15 +1346,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B39" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F39">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G39">
         <v>11</v>
@@ -1347,15 +1366,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B40" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F40">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G40">
         <v>10</v>
@@ -1364,18 +1383,18 @@
         <v>4.99</v>
       </c>
       <c r="I40" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B41" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F41">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G41">
         <v>9</v>
@@ -1387,15 +1406,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B42" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F42">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G42">
         <v>8</v>
@@ -1407,7 +1426,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>29</v>
       </c>
@@ -1415,7 +1434,7 @@
         <v>31</v>
       </c>
       <c r="F43">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G43">
         <v>7</v>
@@ -1427,15 +1446,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B44" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F44">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G44">
         <v>6</v>
@@ -1447,15 +1466,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B45" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F45">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G45">
         <v>5</v>
@@ -1467,15 +1486,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B46" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F46">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G46">
         <v>4</v>
@@ -1487,7 +1506,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>32</v>
       </c>
@@ -1495,7 +1514,7 @@
         <v>34</v>
       </c>
       <c r="F47">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G47">
         <v>3</v>
@@ -1507,7 +1526,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>32</v>
       </c>
@@ -1515,7 +1534,7 @@
         <v>34</v>
       </c>
       <c r="F48">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G48">
         <v>2</v>
@@ -1527,7 +1546,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>32</v>
       </c>
@@ -1535,187 +1554,167 @@
         <v>34</v>
       </c>
       <c r="F49">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H49" s="1">
         <v>4.99</v>
       </c>
       <c r="I49" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B50" t="s">
-        <v>34</v>
-      </c>
-      <c r="F50">
-        <v>49</v>
-      </c>
-      <c r="G50">
-        <v>0</v>
-      </c>
-      <c r="H50" s="1">
-        <v>4.99</v>
-      </c>
-      <c r="I50" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="H50" s="1"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B51" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H51" s="1"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B52" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H52" s="1"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B53" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H53" s="1"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B54" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H54" s="1"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>38</v>
       </c>
       <c r="B55" t="s">
+        <v>52</v>
+      </c>
+      <c r="H55" s="1"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>39</v>
+      </c>
+      <c r="B56" t="s">
+        <v>42</v>
+      </c>
+      <c r="H56" s="1"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>40</v>
+      </c>
+      <c r="B57" t="s">
+        <v>43</v>
+      </c>
+      <c r="H57" s="1"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58">
         <v>41</v>
       </c>
-      <c r="H55" s="1"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>38</v>
-      </c>
-      <c r="B56" t="s">
-        <v>52</v>
-      </c>
-      <c r="H56" s="1"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>39</v>
-      </c>
-      <c r="B57" t="s">
+      <c r="B58" t="s">
+        <v>44</v>
+      </c>
+      <c r="H58" s="1"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59">
         <v>42</v>
       </c>
-      <c r="H57" s="1"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>40</v>
-      </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
+        <v>45</v>
+      </c>
+      <c r="H59" s="1"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60">
         <v>43</v>
       </c>
-      <c r="H58" s="1"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>41</v>
-      </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
+        <v>46</v>
+      </c>
+      <c r="H60" s="1"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A61">
         <v>44</v>
       </c>
-      <c r="H59" s="1"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>42</v>
-      </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
+        <v>47</v>
+      </c>
+      <c r="H61" s="1"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62">
         <v>45</v>
       </c>
-      <c r="H60" s="1"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>43</v>
-      </c>
-      <c r="B61" t="s">
+      <c r="B62" t="s">
+        <v>48</v>
+      </c>
+      <c r="H62" s="1"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63">
         <v>46</v>
       </c>
-      <c r="H61" s="1"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>44</v>
-      </c>
-      <c r="B62" t="s">
+      <c r="B63" t="s">
+        <v>49</v>
+      </c>
+      <c r="H63" s="1"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64">
         <v>47</v>
       </c>
-      <c r="H62" s="1"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>45</v>
-      </c>
-      <c r="B63" t="s">
+      <c r="B64" t="s">
+        <v>50</v>
+      </c>
+      <c r="H64" s="1"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A65">
         <v>48</v>
       </c>
-      <c r="H63" s="1"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>46</v>
-      </c>
-      <c r="B64" t="s">
-        <v>49</v>
-      </c>
-      <c r="H64" s="1"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>47</v>
-      </c>
       <c r="B65" t="s">
+        <v>51</v>
+      </c>
+      <c r="H65" s="1"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A66">
         <v>50</v>
       </c>
-      <c r="H65" s="1"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>48</v>
-      </c>
       <c r="B66" t="s">
-        <v>51</v>
-      </c>
-      <c r="H66" s="1"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <v>50</v>
-      </c>
-      <c r="B67" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Hardcoded and Fixed Grocery Page
Hardcoded the names and pictures of each grocery item, added the button
dropdown, and fixed the pictures in the image file to all the same
format: lower case and spaces where needed.  Also added the picture
locations to the ingredients excel file for easy database entry.
Created two sets of buttons to see which one works better.  Could not
find a way to make the two red buttons expand the width of their
thumbnail container.
</commit_message>
<xml_diff>
--- a/documentation/ingredients.xlsx
+++ b/documentation/ingredients.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="108">
   <si>
     <t>ingredient_id</t>
   </si>
@@ -201,6 +201,189 @@
   </si>
   <si>
     <t>avocados</t>
+  </si>
+  <si>
+    <t>images</t>
+  </si>
+  <si>
+    <t>img/parmesan cheese</t>
+  </si>
+  <si>
+    <t>img/garlic salt</t>
+  </si>
+  <si>
+    <t>img/brown sugar</t>
+  </si>
+  <si>
+    <t>img/lemon juice</t>
+  </si>
+  <si>
+    <t>img/sea salt</t>
+  </si>
+  <si>
+    <t>img/red pepper flakes</t>
+  </si>
+  <si>
+    <t>img/bay leaf</t>
+  </si>
+  <si>
+    <t>img/paprika</t>
+  </si>
+  <si>
+    <t>img/oregano leaves</t>
+  </si>
+  <si>
+    <t>img/cornmeal</t>
+  </si>
+  <si>
+    <t>img/instant yeast</t>
+  </si>
+  <si>
+    <t>img/salt</t>
+  </si>
+  <si>
+    <t>img/bread</t>
+  </si>
+  <si>
+    <t>img/blue cheese</t>
+  </si>
+  <si>
+    <t>img/onion</t>
+  </si>
+  <si>
+    <t>img/celery</t>
+  </si>
+  <si>
+    <t>img/potatoe</t>
+  </si>
+  <si>
+    <t>img/dr. pepper</t>
+  </si>
+  <si>
+    <t>img/chipotle peppers</t>
+  </si>
+  <si>
+    <t>img/pork shoulder</t>
+  </si>
+  <si>
+    <t>img/thyme</t>
+  </si>
+  <si>
+    <t>img/carrot</t>
+  </si>
+  <si>
+    <t>img/mayonnaise</t>
+  </si>
+  <si>
+    <t>img/hot sauce</t>
+  </si>
+  <si>
+    <t>img/pepper jack cheese</t>
+  </si>
+  <si>
+    <t>img/chicken</t>
+  </si>
+  <si>
+    <t>img/milk</t>
+  </si>
+  <si>
+    <t>img/flour</t>
+  </si>
+  <si>
+    <t>img/cilantro</t>
+  </si>
+  <si>
+    <t>img/lime juice</t>
+  </si>
+  <si>
+    <t>img/avocados</t>
+  </si>
+  <si>
+    <t>img/garlic</t>
+  </si>
+  <si>
+    <t>img/elbow macaroni</t>
+  </si>
+  <si>
+    <t>img/rosemary</t>
+  </si>
+  <si>
+    <t>img/pepper</t>
+  </si>
+  <si>
+    <t>img/olive oil</t>
+  </si>
+  <si>
+    <t>img/tortilla chips</t>
+  </si>
+  <si>
+    <t>img/cheddar cheese</t>
+  </si>
+  <si>
+    <t>img/cream cheese</t>
+  </si>
+  <si>
+    <t>img/butter</t>
+  </si>
+  <si>
+    <t>img/sourdough bread</t>
+  </si>
+  <si>
+    <t>img/jalapeno peppers</t>
+  </si>
+  <si>
+    <t>img/water</t>
+  </si>
+  <si>
+    <t>img/ground coffee</t>
+  </si>
+  <si>
+    <t>img/half-and-half</t>
+  </si>
+  <si>
+    <r>
+      <t>same as salt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> img/salt</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>same as Yukon Potatoes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> img/potatoe</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>same as paprika</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> img/paprika</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -210,8 +393,16 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -239,9 +430,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -556,10 +748,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F44" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,10 +759,11 @@
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" customWidth="1"/>
+    <col min="9" max="9" width="29.7109375" customWidth="1"/>
+    <col min="10" max="10" width="34.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -589,8 +782,11 @@
       <c r="I1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -609,8 +805,11 @@
       <c r="I2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -629,8 +828,11 @@
       <c r="I3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -649,8 +851,11 @@
       <c r="I4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -669,8 +874,11 @@
       <c r="I5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -689,8 +897,11 @@
       <c r="I6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -709,8 +920,11 @@
       <c r="I7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -729,8 +943,11 @@
       <c r="I8" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -749,8 +966,11 @@
       <c r="I9" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -769,8 +989,11 @@
       <c r="I10" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
@@ -789,8 +1012,11 @@
       <c r="I11" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -809,8 +1035,11 @@
       <c r="I12" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>8</v>
       </c>
@@ -829,8 +1058,11 @@
       <c r="I13" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>9</v>
       </c>
@@ -849,8 +1081,11 @@
       <c r="I14" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>10</v>
       </c>
@@ -869,8 +1104,11 @@
       <c r="I15" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>11</v>
       </c>
@@ -889,8 +1127,11 @@
       <c r="I16" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>11</v>
       </c>
@@ -909,8 +1150,11 @@
       <c r="I17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>11</v>
       </c>
@@ -929,8 +1173,11 @@
       <c r="I18" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>11</v>
       </c>
@@ -949,8 +1196,11 @@
       <c r="I19" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>12</v>
       </c>
@@ -969,8 +1219,11 @@
       <c r="I20" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>13</v>
       </c>
@@ -989,8 +1242,11 @@
       <c r="I21" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>13</v>
       </c>
@@ -1009,8 +1265,11 @@
       <c r="I22" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>13</v>
       </c>
@@ -1029,8 +1288,11 @@
       <c r="I23" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>13</v>
       </c>
@@ -1049,8 +1311,11 @@
       <c r="I24" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>14</v>
       </c>
@@ -1069,8 +1334,11 @@
       <c r="I25" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>14</v>
       </c>
@@ -1089,8 +1357,11 @@
       <c r="I26" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>15</v>
       </c>
@@ -1109,8 +1380,11 @@
       <c r="I27" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>16</v>
       </c>
@@ -1129,8 +1403,11 @@
       <c r="I28" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>16</v>
       </c>
@@ -1149,8 +1426,11 @@
       <c r="I29" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>17</v>
       </c>
@@ -1169,8 +1449,11 @@
       <c r="I30" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J30" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>17</v>
       </c>
@@ -1189,8 +1472,11 @@
       <c r="I31" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J31" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>18</v>
       </c>
@@ -1209,8 +1495,11 @@
       <c r="I32" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J32" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>19</v>
       </c>
@@ -1229,8 +1518,11 @@
       <c r="I33" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J33" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>21</v>
       </c>
@@ -1249,8 +1541,11 @@
       <c r="I34" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J34" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>21</v>
       </c>
@@ -1269,8 +1564,11 @@
       <c r="I35" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J35" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>22</v>
       </c>
@@ -1289,8 +1587,11 @@
       <c r="I36" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J36" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>23</v>
       </c>
@@ -1309,8 +1610,11 @@
       <c r="I37" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J37" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>24</v>
       </c>
@@ -1329,8 +1633,11 @@
       <c r="I38" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J38" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>25</v>
       </c>
@@ -1349,8 +1656,11 @@
       <c r="I39" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J39" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>26</v>
       </c>
@@ -1369,8 +1679,11 @@
       <c r="I40" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J40" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>27</v>
       </c>
@@ -1389,8 +1702,11 @@
       <c r="I41" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J41" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>28</v>
       </c>
@@ -1409,8 +1725,11 @@
       <c r="I42" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J42" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>29</v>
       </c>
@@ -1429,8 +1748,11 @@
       <c r="I43" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J43" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>29</v>
       </c>
@@ -1449,8 +1771,11 @@
       <c r="I44" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J44" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>30</v>
       </c>
@@ -1469,8 +1794,11 @@
       <c r="I45" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J45" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>31</v>
       </c>
@@ -1489,8 +1817,11 @@
       <c r="I46" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J46" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>32</v>
       </c>
@@ -1509,8 +1840,11 @@
       <c r="I47" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J47" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>32</v>
       </c>
@@ -1529,8 +1863,11 @@
       <c r="I48" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J48" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>32</v>
       </c>
@@ -1549,8 +1886,11 @@
       <c r="I49" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J49" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>32</v>
       </c>
@@ -1569,8 +1909,11 @@
       <c r="I50" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J50" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>33</v>
       </c>
@@ -1579,7 +1922,7 @@
       </c>
       <c r="H51" s="1"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>35</v>
       </c>
@@ -1588,7 +1931,7 @@
       </c>
       <c r="H52" s="1"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>36</v>
       </c>
@@ -1597,7 +1940,7 @@
       </c>
       <c r="H53" s="1"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>37</v>
       </c>
@@ -1606,7 +1949,7 @@
       </c>
       <c r="H54" s="1"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>38</v>
       </c>
@@ -1615,7 +1958,7 @@
       </c>
       <c r="H55" s="1"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>38</v>
       </c>
@@ -1624,7 +1967,7 @@
       </c>
       <c r="H56" s="1"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>39</v>
       </c>
@@ -1633,7 +1976,7 @@
       </c>
       <c r="H57" s="1"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>40</v>
       </c>
@@ -1642,7 +1985,7 @@
       </c>
       <c r="H58" s="1"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>41</v>
       </c>
@@ -1651,7 +1994,7 @@
       </c>
       <c r="H59" s="1"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>42</v>
       </c>
@@ -1660,7 +2003,7 @@
       </c>
       <c r="H60" s="1"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>43</v>
       </c>
@@ -1669,7 +2012,7 @@
       </c>
       <c r="H61" s="1"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>44</v>
       </c>
@@ -1678,7 +2021,7 @@
       </c>
       <c r="H62" s="1"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>45</v>
       </c>
@@ -1687,7 +2030,7 @@
       </c>
       <c r="H63" s="1"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>46</v>
       </c>
@@ -1724,5 +2067,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>